<commit_message>
add of the python script and modification of the excel file
</commit_message>
<xml_diff>
--- a/Excel_models.xlsx
+++ b/Excel_models.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doria\Desktop\Master_Benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3474BF26-6CB6-461B-A094-87C1FFB0A074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{741C0B17-0CFD-4B21-9EBA-F09DF3E81E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BACDE896-C79E-4177-B680-D464181B5ACC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Excel_models" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>deepseek R1</t>
   </si>
@@ -195,6 +195,27 @@
   </si>
   <si>
     <t>nemotron-mini:4b</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>farnaz</t>
+  </si>
+  <si>
+    <t>matevz</t>
+  </si>
+  <si>
+    <t>dorian</t>
+  </si>
+  <si>
+    <t>ali</t>
+  </si>
+  <si>
+    <t>gio</t>
+  </si>
+  <si>
+    <t>raiko</t>
   </si>
 </sst>
 </file>
@@ -589,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574C7515-91A7-4D20-8765-2805C1D77A35}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,6 +631,9 @@
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
@@ -623,7 +647,9 @@
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
@@ -637,7 +663,9 @@
       <c r="C3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -651,7 +679,9 @@
       <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
@@ -665,7 +695,9 @@
       <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
@@ -679,7 +711,9 @@
       <c r="C6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
@@ -693,7 +727,9 @@
       <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
@@ -707,7 +743,9 @@
       <c r="C8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
@@ -721,7 +759,9 @@
       <c r="C9" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -733,6 +773,9 @@
       <c r="C10" t="s">
         <v>50</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -744,7 +787,9 @@
       <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
@@ -758,7 +803,9 @@
       <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
@@ -772,7 +819,9 @@
       <c r="C13" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
@@ -786,6 +835,9 @@
       <c r="C14" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -797,6 +849,9 @@
       <c r="C15" t="s">
         <v>46</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -808,8 +863,11 @@
       <c r="C16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -819,8 +877,11 @@
       <c r="C17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -830,8 +891,11 @@
       <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D18" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -841,8 +905,11 @@
       <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="D19" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -852,8 +919,11 @@
       <c r="C20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -863,8 +933,11 @@
       <c r="C21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -874,8 +947,11 @@
       <c r="C22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -885,15 +961,18 @@
       <c r="C23" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
     </row>

</xml_diff>

<commit_message>
finialisation of the code
</commit_message>
<xml_diff>
--- a/Excel_models.xlsx
+++ b/Excel_models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doria\Desktop\Master_Benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{741C0B17-0CFD-4B21-9EBA-F09DF3E81E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82260E2-FE76-4B10-A656-0A2907C4C82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BACDE896-C79E-4177-B680-D464181B5ACC}"/>
+    <workbookView xWindow="5040" yWindow="2436" windowWidth="17280" windowHeight="8880" xr2:uid="{BACDE896-C79E-4177-B680-D464181B5ACC}"/>
   </bookViews>
   <sheets>
     <sheet name="Excel_models" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>deepseek R1</t>
   </si>
@@ -44,9 +44,6 @@
     <t>gemma 3</t>
   </si>
   <si>
-    <t>embedding gemma</t>
-  </si>
-  <si>
     <t>llama 3,2</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>1,7B</t>
   </si>
   <si>
-    <t>0,3B</t>
-  </si>
-  <si>
     <t>8B</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
   </si>
   <si>
     <t>gemma3:4b</t>
-  </si>
-  <si>
-    <t>embeddinggemma:latest</t>
   </si>
   <si>
     <t>qwen3:0.6b</t>
@@ -610,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574C7515-91A7-4D20-8765-2805C1D77A35}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,346 +614,332 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>